<commit_message>
Grafico da área criado
</commit_message>
<xml_diff>
--- a/PlanilhaMec.xlsx
+++ b/PlanilhaMec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Excel Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBD5738-4E54-4EF0-AFFB-638A3F011110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D3B32D-DB1C-4EC2-BD28-5D25D6DC4F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{255CFAC6-715B-4C6B-AC80-5626B26B3EDB}"/>
   </bookViews>
@@ -628,20 +628,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -740,7 +726,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1134,20 +1120,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1318,6 +1290,544 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Área das Mesas</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$A$4:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$D$4:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>00.000</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>11175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11212.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11205.04</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11197.56</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11145.199999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11175</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11205</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11160.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11220</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11235</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11235</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11235</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11227.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11227.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11205.04</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11235</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11235</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE17-4CED-B4D5-A78CF755E6C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="474711944"/>
+        <c:axId val="474710632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="474711944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Mesas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474710632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="474710632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="11300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Areas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="00.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474711944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1398,6 +1908,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2404,20 +2954,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>400050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2432,8 +3485,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3933825" y="28575"/>
-          <a:ext cx="4210050" cy="419100"/>
+          <a:off x="38100" y="200025"/>
+          <a:ext cx="4210050" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2541,6 +3594,105 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Retângulo: Cantos Arredondados 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E91EAB5-6779-43AB-A447-8C5CF5607D6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9058275" y="476250"/>
+          <a:ext cx="1666875" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2000" b="1"/>
+            <a:t>Histogramas</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F2CEC2B-AF8F-433E-92CD-1F392E21F4F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2861,10 +4013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F8B7C0-8265-4FED-9DD6-2B21D30538D2}">
-  <dimension ref="A3:D29"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,6 +4027,7 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Realizando os calculos da propagação de erros
</commit_message>
<xml_diff>
--- a/PlanilhaMec.xlsx
+++ b/PlanilhaMec.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Excel Estudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7833F9B-EAC1-48BF-942E-523861332894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DDDDB9-2262-45B1-B8E4-E057BB428762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{255CFAC6-715B-4C6B-AC80-5626B26B3EDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Gráficos" sheetId="1" r:id="rId1"/>
+    <sheet name="Cálculos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Mesa</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Calculo da área(L media x C media):</t>
+  </si>
+  <si>
+    <t>Desvio Padrão Área (cm²)</t>
+  </si>
+  <si>
+    <t>Erro da Área</t>
   </si>
 </sst>
 </file>
@@ -129,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -141,6 +147,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,7 +501,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$26</c:f>
+              <c:f>Gráficos!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -576,7 +585,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$C$2:$C$26</c:f>
+              <c:f>Gráficos!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1044,7 +1053,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$26</c:f>
+              <c:f>Gráficos!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1464,7 +1473,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Planilha1!$A$2:$A$26</c:f>
+              <c:f>Gráficos!$A$2:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1548,7 +1557,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$D$2:$D$26</c:f>
+              <c:f>Gráficos!$D$2:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>00,000</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1986,7 +1995,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$C$1</c:f>
+              <c:f>Gráficos!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2019,7 +2028,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Planilha1!$C$2:$C$26</c:f>
+              <c:f>Gráficos!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2103,7 +2112,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Planilha1!$B$2:$B$26</c:f>
+              <c:f>Gráficos!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -4637,16 +4646,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4661,7 +4670,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10086975" y="28574"/>
+          <a:off x="8286750" y="0"/>
           <a:ext cx="1228725" cy="333376"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -4778,15 +4787,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1181101</xdr:colOff>
+      <xdr:colOff>1657351</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4801,8 +4810,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6019801" y="104775"/>
-          <a:ext cx="1219200" cy="333376"/>
+          <a:off x="6496051" y="95250"/>
+          <a:ext cx="1352549" cy="333376"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -4836,6 +4845,123 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo: Cantos Arredondados 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE962AC2-BC82-4E6B-B29F-401804EE8C57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4972051" y="2571750"/>
+          <a:ext cx="2543174" cy="333376"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1"/>
+            <a:t>Propagação</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0"/>
+            <a:t> de Erro da Área</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1400" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1273821</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929ED7BE-E71D-4E16-B59E-57DC40C43DEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="18015" t="10035" r="20711" b="19089"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7639050" y="2466976"/>
+          <a:ext cx="2950221" cy="542924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5170,8 +5296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F8B7C0-8265-4FED-9DD6-2B21D30538D2}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5591,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57DE712F-C8CB-45CD-89E8-DFE62483C883}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5915,7 +6041,7 @@
         <v>11160.1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5930,7 +6056,7 @@
         <v>11220</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5944,8 +6070,15 @@
         <f t="shared" si="0"/>
         <v>11235</v>
       </c>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5">
+        <f>H7</f>
+        <v>48.46035022572584</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5959,8 +6092,15 @@
         <f t="shared" si="0"/>
         <v>11235</v>
       </c>
+      <c r="F19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5">
+        <f>G7</f>
+        <v>11203.2176</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5974,8 +6114,15 @@
         <f t="shared" si="0"/>
         <v>11235</v>
       </c>
+      <c r="F20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="5">
+        <f>SQRT((H5/G5)^2 + (H6/G6)^2)*G7</f>
+        <v>50.674830212554852</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5990,7 +6137,7 @@
         <v>11227.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -6005,7 +6152,7 @@
         <v>11227.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -6020,7 +6167,7 @@
         <v>11205.04</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -6035,7 +6182,7 @@
         <v>11235</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -6050,7 +6197,7 @@
         <v>11250</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>

</xml_diff>